<commit_message>
cosmetic + add time with 02
</commit_message>
<xml_diff>
--- a/analytics/program_time_and_size.xlsx
+++ b/analytics/program_time_and_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniil\Documents\Proggers1337\Hash_table_analysis\analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC76C2D8-97A2-4FDC-A9F1-CFF0AD4CC128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE78431B-8E8F-4AB8-868F-7A4F092B923B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,120 +244,164 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>41836</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Рисунок 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{104FD09A-5E3B-40DC-9077-85490F8EE326}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="182880"/>
+          <a:ext cx="1615440" cy="590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Рисунок 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9543AFF2-ECCD-46FC-8BBF-39C12EAECCB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="914400"/>
+          <a:ext cx="1630680" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Рисунок 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F02B14-565D-4553-8012-6EBC0E4615E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="1645921"/>
+          <a:ext cx="1615440" cy="586740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57076</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D09437C-7E7D-4BE5-B676-E3AEC298609C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4693920" y="198120"/>
-          <a:ext cx="1645920" cy="590476"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>89455</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A69CBD4-A9CC-4AB2-B07B-F88FCDF01B39}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4716780" y="914400"/>
-          <a:ext cx="1623060" cy="638095"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>60884</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A500FBB-7B31-4531-B457-3E659EC1C2D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+      <xdr:rowOff>70408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Рисунок 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46808D72-0EEC-438B-A562-6297C4F76740}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -365,7 +409,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4716780" y="2377440"/>
-          <a:ext cx="1638300" cy="609524"/>
+          <a:ext cx="1623060" cy="619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -385,23 +429,23 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>41836</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0DA3FFD-0C2E-4C20-A2BC-C20DE002ED53}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+      <xdr:rowOff>70408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Рисунок 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52D764F-89C2-42B8-8B4B-E78C13C09FBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -409,7 +453,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4716780" y="3108960"/>
-          <a:ext cx="1623060" cy="590476"/>
+          <a:ext cx="1623060" cy="619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -428,32 +472,76 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Рисунок 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F6BACDB-BDD7-4D82-A4EF-5CA8466148FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="3840480"/>
+          <a:ext cx="1615440" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>51360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5887B3E8-5EF0-49F2-A204-832D1630DA5B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4716780" y="3840480"/>
-          <a:ext cx="1615440" cy="600000"/>
+        <xdr:cNvPr id="16" name="Рисунок 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70C4B1E0-9AB2-47AF-B9DF-9CE83E44A6E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="3840480"/>
+          <a:ext cx="1607820" cy="600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -466,82 +554,170 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CE7FA7-EF4F-4649-899F-0C2D6896DA8A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6941820" y="3840481"/>
-          <a:ext cx="1600200" cy="624840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Рисунок 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFAFD1B2-5CEE-4066-BC5D-F36713359B3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="3108960"/>
+          <a:ext cx="1600200" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Рисунок 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C343CF9-1C22-4D78-8D2B-809A0220F54E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="2377440"/>
+          <a:ext cx="1607820" cy="594360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>60884</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Рисунок 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43201BAA-F273-45B2-9C4F-EA28F7BC440F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4716780" y="1645920"/>
-          <a:ext cx="1630680" cy="609524"/>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Рисунок 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78BDA959-7482-476B-9BCD-1DD5C4956922}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="1645920"/>
+          <a:ext cx="1607820" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>51360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Рисунок 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30BFF82E-B776-46E0-820D-8E6EAF439B1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="914400"/>
+          <a:ext cx="1600200" cy="600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -561,23 +737,23 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>79931</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5655122A-119A-43A2-BB4D-28B1CA5E625A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Рисунок 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A087A37-9140-47B7-B1F2-A9B79567F606}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -585,7 +761,1063 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6941820" y="182880"/>
-          <a:ext cx="1607820" cy="628571"/>
+          <a:ext cx="1607820" cy="586740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Рисунок 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC2BD4A6-CE34-4CAE-888D-B1BD709543AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="4937760"/>
+          <a:ext cx="1600200" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Рисунок 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E4F227-6DD7-47DB-A995-191BDB554449}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="4937760"/>
+          <a:ext cx="1630680" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>51360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Рисунок 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8AFE744-4832-4BAA-AB9D-344A868BD503}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="5669280"/>
+          <a:ext cx="1623060" cy="600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>70408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Рисунок 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD721311-9091-414C-B5C2-F102E86C695B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="5669280"/>
+          <a:ext cx="1607820" cy="619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>22789</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Рисунок 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31520213-EBCE-492B-945D-76468DB0907F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="6400800"/>
+          <a:ext cx="1607820" cy="571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Рисунок 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{824D4E3E-0227-4C9B-9832-531A28175378}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="6400800"/>
+          <a:ext cx="1623060" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>3741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Рисунок 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EAD759F-5EE3-4A61-A702-D0D781350476}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="7132320"/>
+          <a:ext cx="1615440" cy="552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>13265</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Рисунок 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5855D9DD-2FA5-4F6E-A7E4-E438C8F72143}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="7132320"/>
+          <a:ext cx="1607820" cy="561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>41831</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Рисунок 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFFDA8D7-E15F-4645-9DCE-692C175DDC84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="7825740"/>
+          <a:ext cx="1615440" cy="628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Рисунок 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C13DC5F9-1816-4BB6-8BA3-401304AF7991}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="7863840"/>
+          <a:ext cx="1623060" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>51360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Рисунок 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBA86A6-843A-41DC-8B1D-1AA92B0EAA4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="8595360"/>
+          <a:ext cx="1630680" cy="600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>98979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Рисунок 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E202C281-453B-43F6-8D21-4F918CF27BC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="8595360"/>
+          <a:ext cx="1615440" cy="647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Рисунок 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF2296B1-945C-4C64-963A-8AE105A7D50F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="13533120"/>
+          <a:ext cx="1615440" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>41836</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Рисунок 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771C879B-589C-4E1D-80DD-9EF7189834E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="13533120"/>
+          <a:ext cx="1630680" cy="590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Рисунок 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E5AC351-EB28-4212-A326-4C63205D81BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="12801600"/>
+          <a:ext cx="1623060" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Рисунок 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE1AEFA4-7DA7-4209-B938-0BA5FD0AF4FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="12801600"/>
+          <a:ext cx="1600200" cy="586740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Рисунок 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD8FBE69-EA1C-42E3-8A15-58DB26501920}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="12070080"/>
+          <a:ext cx="1615440" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Рисунок 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8903418C-320E-43D3-9C5E-59B1DC64BFAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="12070080"/>
+          <a:ext cx="1623060" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Рисунок 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{133ED908-D5E4-4E0F-92DA-1FF31DB245AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="11338560"/>
+          <a:ext cx="1630680" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Рисунок 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E77151E-9E80-452C-B32F-A2EF2C5D6624}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="11338560"/>
+          <a:ext cx="1607820" cy="624840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Рисунок 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DDA0876-1AF0-4878-B9E3-780E76015335}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="10607040"/>
+          <a:ext cx="1630680" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>32312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Рисунок 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCE13AC0-FD53-45D2-8244-552212954E89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="10607040"/>
+          <a:ext cx="1615440" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>60884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Рисунок 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58939E95-33C5-4A7D-8D09-5BBF3E27E697}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6941820" y="9875520"/>
+          <a:ext cx="1607820" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>51360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Рисунок 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E75D0DA-1DA8-45A1-BC07-855B1005DE65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4716780" y="9875520"/>
+          <a:ext cx="1623060" cy="600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -862,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,9 +2139,6 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
-        <v>5.2999999999999999E-2</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">

</xml_diff>